<commit_message>
add ssd300 voc and coco config
</commit_message>
<xml_diff>
--- a/records/experiments.xlsx
+++ b/records/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\adversarialAttack\paper\aaod\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEE1C4C-DC0D-44E9-BB5C-D6FB17F95985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65890BF0-4A0B-481C-A32E-006FBA30DFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{616F5F3B-DB8B-4E6E-962A-D65942DCE50F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>1D16H</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,14 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2D 16H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FLOPs / 1e9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -72,6 +64,106 @@
   </si>
   <si>
     <t>coco2014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-R101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voc0712</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPU_NUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU_US</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU_SY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load average</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTX 3070</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTX 3060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.09, 1.82, 1.09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7392, 6490</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPU_Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memory-Usage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D16H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~7000+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FR-R101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTX 3060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D14H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.23, 1.72, 0.86</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000, 8400</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -96,6 +188,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
@@ -103,8 +196,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="2"/>
@@ -137,11 +229,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,103 +549,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4521C526-7D1B-4483-9848-A6F371A5B763}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3814</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="G3" s="1">
         <v>12</v>
       </c>
-      <c r="E3" s="1">
-        <v>5705</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
         <v>7.6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="J4" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="J6" s="1">
+        <v>13</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change ssd voc batch_size to 4
</commit_message>
<xml_diff>
--- a/records/experiments.xlsx
+++ b/records/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\adversarialAttack\paper\aaod\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65890BF0-4A0B-481C-A32E-006FBA30DFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E611AFB9-3161-4400-8C3B-1476C8EB4FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{616F5F3B-DB8B-4E6E-962A-D65942DCE50F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>1D16H</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -164,6 +164,30 @@
   </si>
   <si>
     <t>10000, 8400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSD300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTX 3070</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6D 9H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTX 3060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12G</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -552,7 +576,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -794,8 +818,56 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1">
+        <v>8000</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>24</v>
+      </c>
+    </row>
     <row r="9" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add dcn_attack and update componets
</commit_message>
<xml_diff>
--- a/records/experiments.xlsx
+++ b/records/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\adversarialAttack\paper\aaod\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E611AFB9-3161-4400-8C3B-1476C8EB4FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8BA1A2-FB30-41F6-9C27-606EC0C84DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{616F5F3B-DB8B-4E6E-962A-D65942DCE50F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>1D16H</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -188,6 +188,22 @@
   </si>
   <si>
     <t>12G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D 7H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.08, 1.93, 1.14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11218, 11218</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -249,7 +265,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -257,6 +273,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4521C526-7D1B-4483-9848-A6F371A5B763}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -863,9 +885,26 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
       <c r="G8" s="1">
         <v>24</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -876,6 +915,11 @@
     <row r="14" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>